<commit_message>
Actualizacióin del repositorio global con lo de trabajado en LENOVO 2024-12-12
</commit_message>
<xml_diff>
--- a/ChatGPT.xlsx
+++ b/ChatGPT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios\Torddis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453FD79D-BCAD-4C77-A957-1AF1DD88CFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898556BF-5632-4388-8EDF-26B2A535CF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18B9FF24-9432-4BD0-9DAC-67AA956D0EBC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{18B9FF24-9432-4BD0-9DAC-67AA956D0EBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="42">
   <si>
     <t>Edad del tutor</t>
   </si>
@@ -161,17 +159,14 @@
     <t>P12</t>
   </si>
   <si>
-    <t>Nota:</t>
-  </si>
-  <si>
-    <t>En la escala de Likert (del 1: totalmente en desacuerdo al 5: totalmente de acuerdo)</t>
+    <t>Encuestado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,13 +193,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -233,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -304,20 +292,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,9 +330,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,16 +665,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A15A289-1075-41AD-BF59-4D5ABC21B271}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:R14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="192" x14ac:dyDescent="0.3">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:18" ht="192">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -751,7 +729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="26.4">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -807,7 +785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="26.4">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -863,7 +841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -919,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="26.4">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -975,7 +953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="26.4">
       <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
@@ -1031,7 +1009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="39.6">
       <c r="A7" s="10" t="s">
         <v>33</v>
       </c>
@@ -1087,7 +1065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="26.4">
       <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
@@ -1143,7 +1121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18">
       <c r="A9" s="10" t="s">
         <v>36</v>
       </c>
@@ -1199,7 +1177,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18">
       <c r="A10" s="11" t="s">
         <v>37</v>
       </c>
@@ -1255,7 +1233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18">
       <c r="A11" s="11" t="s">
         <v>38</v>
       </c>
@@ -1311,7 +1289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="26.4">
       <c r="A12" s="11" t="s">
         <v>39</v>
       </c>
@@ -1367,7 +1345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" ht="39.6">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -1423,33 +1401,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="12"/>
+    <row r="15" spans="1:18">
+      <c r="B15">
+        <f>MIN(B2:B13)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16">
+        <f>MAX(B2:B13)</f>
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B14:Q14"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>